<commit_message>
Test Order is Completed
</commit_message>
<xml_diff>
--- a/TestData/Test_Data.xlsx
+++ b/TestData/Test_Data.xlsx
@@ -1,68 +1,174 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tejas\Class Project\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05501FA-9BBF-4EA8-89CF-EC9748B8FBA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>User Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Confirm Password</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Actual Result</t>
+  </si>
+  <si>
+    <t>Test Pass/Fail</t>
+  </si>
+  <si>
+    <t>Unknown Owner</t>
+  </si>
+  <si>
+    <t>Unknown2023@gmail.com</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Order Data</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>Card No</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Kim</t>
+  </si>
+  <si>
+    <t>Pune, Maharashtra, India</t>
+  </si>
+  <si>
+    <t>Jong</t>
+  </si>
+  <si>
+    <t>Kim Jong</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="10.5"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="9.8000000000000007"/>
+      <color theme="1"/>
       <name val="JetBrains Mono"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="9.800000000000001"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="10"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <u val="single"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -296,6 +402,56 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -303,154 +459,122 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+  <cellXfs count="34">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -716,165 +840,275 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.140625" customWidth="1" style="5" min="1" max="1"/>
-    <col width="28.7109375" customWidth="1" style="5" min="2" max="3"/>
-    <col width="17" customWidth="1" style="5" min="4" max="4"/>
-    <col width="19.5703125" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
-    <col width="16.7109375" customWidth="1" style="5" min="6" max="6"/>
-    <col width="14.7109375" customWidth="1" style="5" min="7" max="7"/>
-    <col width="14.42578125" customWidth="1" style="5" min="8" max="8"/>
-    <col width="9.140625" customWidth="1" style="5" min="9" max="16384"/>
+    <col min="1" max="1" width="9.140625" style="5" customWidth="1"/>
+    <col min="2" max="3" width="28.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="17" style="5" customWidth="1"/>
+    <col min="5" max="5" width="29" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="22" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A1" s="20" t="inlineStr">
-        <is>
-          <t>No.</t>
-        </is>
-      </c>
-      <c r="B1" s="19" t="inlineStr">
-        <is>
-          <t>User Name</t>
-        </is>
-      </c>
-      <c r="C1" s="19" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="D1" s="19" t="inlineStr">
-        <is>
-          <t>Password</t>
-        </is>
-      </c>
-      <c r="E1" s="21" t="inlineStr">
-        <is>
-          <t>Confirm Password</t>
-        </is>
-      </c>
-      <c r="F1" s="4" t="inlineStr">
-        <is>
-          <t>Expected Result</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Actual Result</t>
-        </is>
-      </c>
-      <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>Test Pass/Fail</t>
-        </is>
+    <row r="1" spans="1:12" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2" ht="18" customHeight="1">
-      <c r="A2" s="6" t="n">
+    <row r="2" spans="1:12" ht="18" customHeight="1">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="inlineStr">
-        <is>
-          <t>Unknown Owner</t>
-        </is>
-      </c>
-      <c r="C2" s="24" t="inlineStr">
-        <is>
-          <t>Unknown2023@gmail.com</t>
-        </is>
-      </c>
-      <c r="D2" s="7" t="n">
+      <c r="B2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="7">
         <v>1234512345</v>
       </c>
-      <c r="E2" s="23" t="n">
+      <c r="E2" s="23">
         <v>1234512345</v>
       </c>
-      <c r="F2" s="15" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-      <c r="G2" s="8" t="inlineStr">
-        <is>
-          <t>Fail</t>
-        </is>
-      </c>
-      <c r="H2" s="7" t="n"/>
+      <c r="F2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="7"/>
     </row>
-    <row r="3" ht="18" customHeight="1">
-      <c r="A3" s="9" t="n">
+    <row r="3" spans="1:12" ht="18" customHeight="1">
+      <c r="A3" s="9">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="inlineStr">
-        <is>
-          <t>Unknown Owner</t>
-        </is>
-      </c>
-      <c r="C3" s="22" t="inlineStr">
-        <is>
-          <t>Unknown2023@gmail.com</t>
-        </is>
-      </c>
-      <c r="D3" s="10" t="n">
+      <c r="B3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="10">
         <v>1234512345</v>
       </c>
-      <c r="E3" s="16" t="n">
+      <c r="E3" s="16">
         <v>1234512345</v>
       </c>
-      <c r="F3" s="16" t="inlineStr">
-        <is>
-          <t>Fail</t>
-        </is>
-      </c>
-      <c r="G3" s="11" t="inlineStr">
-        <is>
-          <t>Fail</t>
-        </is>
-      </c>
-      <c r="H3" s="10" t="n"/>
+      <c r="F3" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="10"/>
     </row>
-    <row r="4">
-      <c r="A4" s="9" t="n">
+    <row r="4" spans="1:12">
+      <c r="A4" s="9">
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="n"/>
-      <c r="C4" s="22" t="n"/>
-      <c r="D4" s="10" t="n"/>
-      <c r="E4" s="16" t="n"/>
-      <c r="F4" s="16" t="n"/>
-      <c r="G4" s="11" t="n"/>
-      <c r="H4" s="10" t="n"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="10"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A5" s="12" t="n">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A5" s="12">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="n"/>
-      <c r="C5" s="18" t="n"/>
-      <c r="D5" s="13" t="n"/>
-      <c r="E5" s="17" t="n"/>
-      <c r="F5" s="17" t="n"/>
-      <c r="G5" s="14" t="n"/>
-      <c r="H5" s="13" t="n"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="13"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" thickBot="1"/>
+    <row r="8" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A8" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="27"/>
+    </row>
+    <row r="9" spans="1:12" ht="21" customHeight="1" thickBot="1">
+      <c r="A9" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="33" customFormat="1">
+      <c r="A10" s="29">
+        <v>1</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="30">
+        <v>9876543210</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="30">
+        <v>412121</v>
+      </c>
+      <c r="G10" s="31">
+        <v>2</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="31">
+        <v>123</v>
+      </c>
+      <c r="J10" s="32">
+        <v>4716108899721050</v>
+      </c>
+      <c r="K10" s="31">
+        <v>2025</v>
+      </c>
+      <c r="L10" s="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="9">
+        <v>2</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="9">
+        <v>3</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="10"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A13" s="12">
+        <v>4</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="13"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:L8"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>